<commit_message>
SO Test Plan, Migration from QARSF to AutomationOrg
</commit_message>
<xml_diff>
--- a/templates/QARSF/AR.xlsx
+++ b/templates/QARSF/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\WS_RSAutomation\rsqasampleproj\templates\QARSF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77389C6F-C24A-4172-83F7-F53E0AFFA2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3AE740-2A1F-4D3C-9B13-B5DD3C3FCC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="300" windowWidth="15375" windowHeight="7875" tabRatio="761" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26670" yWindow="2445" windowWidth="19875" windowHeight="7875" tabRatio="761" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>API Mode</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Packaging Amount</t>
   </si>
   <si>
-    <t>Cust-Dollar WF1 (8)</t>
-  </si>
-  <si>
     <t>Bank Account</t>
   </si>
   <si>
@@ -157,13 +154,22 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>Cust-Dollar WF1</t>
+  </si>
+  <si>
+    <t>a5B41000000PRNXEA4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +196,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,11 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,29 +1025,32 @@
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
       </c>
       <c r="B2">
         <v>450</v>
@@ -1042,14 +1058,17 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2">
         <v>450</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
+      <c r="G2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Migration to Automation-Org/TestCases-maintenance/WIP-RMA TestCases"
</commit_message>
<xml_diff>
--- a/templates/QARSF/AR.xlsx
+++ b/templates/QARSF/AR.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\WS_RSAutomation\rsqasampleproj\templates\QARSF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77389C6F-C24A-4172-83F7-F53E0AFFA2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D875F2-5145-4D41-BC39-20C96BBD358B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="300" windowWidth="15375" windowHeight="7875" tabRatio="761" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26595" yWindow="2010" windowWidth="18330" windowHeight="11385" tabRatio="761" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
-    <sheet name="AddLine" sheetId="2" r:id="rId2"/>
-    <sheet name="FirmAllLines" sheetId="3" r:id="rId3"/>
-    <sheet name="Allocate" sheetId="5" r:id="rId4"/>
-    <sheet name="PickPackShip" sheetId="13" r:id="rId5"/>
-    <sheet name="CreateInvoice" sheetId="18" r:id="rId6"/>
-    <sheet name="CashReceipt" sheetId="21" r:id="rId7"/>
+    <sheet name="AddHeader_ForeignCurr" sheetId="23" r:id="rId2"/>
+    <sheet name="AddLine" sheetId="2" r:id="rId3"/>
+    <sheet name="AddLine_ForeignCurr" sheetId="24" r:id="rId4"/>
+    <sheet name="FirmAllLines" sheetId="3" r:id="rId5"/>
+    <sheet name="Allocate" sheetId="5" r:id="rId6"/>
+    <sheet name="PickPackShip" sheetId="13" r:id="rId7"/>
+    <sheet name="CreateInvoice" sheetId="18" r:id="rId8"/>
+    <sheet name="CashReceipt" sheetId="21" r:id="rId9"/>
+    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="45">
   <si>
     <t>API Mode</t>
   </si>
@@ -135,9 +138,6 @@
     <t>Packaging Amount</t>
   </si>
   <si>
-    <t>Cust-Dollar WF1 (8)</t>
-  </si>
-  <si>
     <t>Bank Account</t>
   </si>
   <si>
@@ -157,13 +157,34 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>Cust-Dollar WF1</t>
+  </si>
+  <si>
+    <t>a5B41000000PRNXEA4</t>
+  </si>
+  <si>
+    <t>BC-INR</t>
+  </si>
+  <si>
+    <t>a5B410000004My9EAE</t>
+  </si>
+  <si>
+    <t>SR-INR</t>
+  </si>
+  <si>
+    <t>a5B410000004My9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +211,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,11 +244,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +534,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +599,141 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D22201-C5D6-472B-8859-9FD3E7767F3C}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>450</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2">
+        <v>450</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6BCBCB-A84A-46BC-A06B-C9A4674BBF49}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E477E4AB-7195-46E9-AE4C-74460C3E66C8}">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -838,7 +1007,280 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C2144E-CB5D-4D95-BAF4-FD830A8B820D}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>40</v>
+      </c>
+      <c r="M3">
+        <v>30</v>
+      </c>
+      <c r="N3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>50</v>
+      </c>
+      <c r="N4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A014ED-6B4B-4C73-85E3-BCAF80680504}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -875,7 +1317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA382408-0CA4-42C9-9A0F-02454DC598A0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -918,7 +1360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3AAA29-D8B0-49CC-98B1-95E06AACF704}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -958,7 +1400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2448C880-E0DE-4186-968F-5BE216A9193B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -999,12 +1441,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,29 +1454,32 @@
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
       </c>
       <c r="B2">
         <v>450</v>
@@ -1042,14 +1487,17 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2">
         <v>450</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
+      <c r="G2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>